<commit_message>
Migrated CMA SW to new Tables Copied CMA SW to Sand Updated CMA to use new template on sand
</commit_message>
<xml_diff>
--- a/Projects/CCBOTTLERSUS/CMA/Data/CMA Compliance Template v0.9.xlsx
+++ b/Projects/CCBOTTLERSUS/CMA/Data/CMA Compliance Template v0.9.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -46,16 +46,124 @@
     <t xml:space="preserve">store_attribute</t>
   </si>
   <si>
+    <t xml:space="preserve">SSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CDE Outside Impulse Zone, Cold Vault</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR&amp;LT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Still</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isotonic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enhanced Water (Vitamin Water)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPI Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_ean_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Target</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7613035738539, 7613035738119, 50189779, 50251797, 7613035220065, 7613034954459, 3800020415009, 7613035058347, 7613035052024, 7613034872630, 50251414, 761303495928</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numerator param 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numerator value 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numerator param 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numerator value 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">denominator param 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">denominator value 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">denominator param 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">denominator value 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United Deliver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">att4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brand_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POWERADE,Bodyarmor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GLACEAU VITAMIN WATER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub_category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enhanced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">region</t>
+  </si>
+  <si>
+    <t xml:space="preserve">program</t>
+  </si>
+  <si>
+    <t xml:space="preserve">channel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">target</t>
+  </si>
+  <si>
     <t xml:space="preserve">SOS SSD</t>
   </si>
   <si>
-    <t xml:space="preserve">SOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CDE Outside Impulse Zone, Cold Vault</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CR&amp;LT</t>
+    <t xml:space="preserve">UNITED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baton Rouge Preferred</t>
   </si>
   <si>
     <t xml:space="preserve">SOS Still</t>
@@ -77,114 +185,6 @@
   </si>
   <si>
     <t xml:space="preserve">SOS Enhanced Water (Vitamin Water)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KPI Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_ean_code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Target</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Visible</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7613035738539, 7613035738119, 50189779, 50251797, 7613035220065, 7613034954459, 3800020415009, 7613035058347, 7613035052024, 7613034872630, 50251414, 761303495928</t>
-  </si>
-  <si>
-    <t xml:space="preserve">numerator param 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">numerator value 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">numerator param 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">numerator value 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">denominator param 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">denominator value 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">denominator param 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">denominator value 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">United Deliver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SSD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">att4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Still</t>
-  </si>
-  <si>
-    <t xml:space="preserve">brand_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POWERADE,Bodyarmor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Isotonic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Energy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Juice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GLACEAU VITAMIN WATER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub_category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enhanced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">region</t>
-  </si>
-  <si>
-    <t xml:space="preserve">program</t>
-  </si>
-  <si>
-    <t xml:space="preserve">channel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">target</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNITED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Baton Rouge Preferred</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enhanced Water (Vitamin Water)</t>
   </si>
   <si>
     <t xml:space="preserve">Baton Rouge Partnership</t>
@@ -481,8 +481,8 @@
   </sheetPr>
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -701,8 +701,8 @@
   </sheetPr>
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -764,13 +764,13 @@
         <v>33</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -781,10 +781,10 @@
         <v>11</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>31</v>
@@ -793,10 +793,10 @@
         <v>32</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -807,10 +807,10 @@
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>31</v>
@@ -822,7 +822,7 @@
         <v>33</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -836,7 +836,7 @@
         <v>33</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>31</v>
@@ -848,7 +848,7 @@
         <v>33</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -862,7 +862,7 @@
         <v>33</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>31</v>
@@ -874,7 +874,7 @@
         <v>33</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -888,7 +888,7 @@
         <v>33</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>31</v>
@@ -900,7 +900,7 @@
         <v>33</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -914,7 +914,7 @@
         <v>33</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>31</v>
@@ -926,7 +926,7 @@
         <v>33</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -937,10 +937,10 @@
         <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>37</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>44</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>31</v>
@@ -952,13 +952,13 @@
         <v>33</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="L9" s="10"/>
     </row>
@@ -981,10 +981,10 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.8866396761134"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.49797570850202"/>
@@ -993,32 +993,32 @@
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>10</v>
@@ -1027,15 +1027,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>10</v>
@@ -1044,15 +1044,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>10</v>
@@ -1061,15 +1061,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>10</v>
@@ -1078,15 +1078,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>10</v>
@@ -1095,15 +1095,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>10</v>
@@ -1112,15 +1112,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>10</v>
@@ -1129,15 +1129,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>10</v>
@@ -1146,12 +1146,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>54</v>
@@ -1163,12 +1163,12 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>54</v>
@@ -1180,12 +1180,12 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>54</v>
@@ -1197,12 +1197,12 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>54</v>
@@ -1214,12 +1214,12 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>54</v>
@@ -1231,12 +1231,12 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>54</v>
@@ -1248,12 +1248,12 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>54</v>
@@ -1265,12 +1265,12 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>54</v>
@@ -1282,12 +1282,12 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>55</v>
@@ -1299,12 +1299,12 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>55</v>
@@ -1316,12 +1316,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>55</v>
@@ -1333,12 +1333,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>55</v>
@@ -1350,12 +1350,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>55</v>
@@ -1367,12 +1367,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C23" s="14" t="s">
         <v>55</v>
@@ -1384,12 +1384,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C24" s="14" t="s">
         <v>55</v>
@@ -1401,12 +1401,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C25" s="14" t="s">
         <v>55</v>

</xml_diff>